<commit_message>
Updates to Average Vehicle Lifetimes, SoCDTtiNtY and BAU Historical New Vehicle Fuel Economy After Lifetime, stemming drop dropping the LDV passenger lifetime from 17 to 13, in line with the US national model. Brings new vehicle sales in line with actual statistics.
</commit_message>
<xml_diff>
--- a/InputData/trans/BHNVFEAL/BAU Historical New Veh Fuel Economy After Lifetime.xlsx
+++ b/InputData/trans/BHNVFEAL/BAU Historical New Veh Fuel Economy After Lifetime.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\California\Models\eps-california\InputData\trans\BHNVFEAL\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="19395" windowHeight="10995" tabRatio="742" firstSheet="10" activeTab="14"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="19395" windowHeight="10995" tabRatio="742" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -38,12 +43,12 @@
     <definedName name="ti_tbl_50">#REF!</definedName>
     <definedName name="ti_tbl_69">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="50">
   <si>
     <t>Sources:</t>
   </si>
@@ -180,9 +185,6 @@
     <t>For on road vehicles, historical data on vehicle efficiency by vintage is used to estimate average fuel economy of retiring vehicles.</t>
   </si>
   <si>
-    <t xml:space="preserve">For example, since a LDV passenger vehicle is assumed to have a life of 17 years, the retiring vehicles in a given year will reflect new vehicle economy </t>
-  </si>
-  <si>
     <t xml:space="preserve">from 18 years prior. </t>
   </si>
   <si>
@@ -191,11 +193,17 @@
   <si>
     <t>Freight</t>
   </si>
+  <si>
+    <t xml:space="preserve">For example, since a LDV passenger vehicle is assumed to have a life of 13 years, the retiring vehicles in a given year will reflect new vehicle economy </t>
+  </si>
+  <si>
+    <t>LDV Lifetime</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="6">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -450,7 +458,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="31">
+  <fills count="32">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -605,6 +613,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1068,7 +1082,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1097,6 +1111,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="153">
     <cellStyle name="20% - Accent1 2" xfId="8"/>
@@ -1390,7 +1405,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1425,7 +1440,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1634,10 +1649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1689,12 +1704,20 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="8" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="22">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -6077,8 +6100,8 @@
   </sheetPr>
   <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="A10:C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10304,7 +10327,7 @@
   <dimension ref="A1:BA55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11238,7 +11261,7 @@
   <dimension ref="A1:BP22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S4" sqref="S4:BA9"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15348,10 +15371,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="B3" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -15399,8 +15422,8 @@
   </sheetPr>
   <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15520,144 +15543,144 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <f>'LDV psg'!B5</f>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!B$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
         <v>1.5777856020187898E-3</v>
       </c>
       <c r="C2">
-        <f>'LDV psg'!C5</f>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!C$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
         <v>1.5777856020187898E-3</v>
       </c>
       <c r="D2">
-        <f>'LDV psg'!D5</f>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!D$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
         <v>1.5777856020187898E-3</v>
       </c>
       <c r="E2">
-        <f>'LDV psg'!E5</f>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!E$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
         <v>1.5777856020187898E-3</v>
       </c>
       <c r="F2">
-        <f>'LDV psg'!F5</f>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!F$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
         <v>1.5777856020187898E-3</v>
       </c>
       <c r="G2">
-        <f>'LDV psg'!G5</f>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!G$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
         <v>1.5777856020187898E-3</v>
       </c>
       <c r="H2">
-        <f>'LDV psg'!H5</f>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!H$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
         <v>1.5777856020187898E-3</v>
       </c>
       <c r="I2">
-        <f>'LDV psg'!I5</f>
-        <v>1.5777856020187898E-3</v>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!I$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.5772719898126412E-3</v>
       </c>
       <c r="J2">
-        <f>'LDV psg'!J5</f>
-        <v>1.5777856020187898E-3</v>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!J$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.5792887696596991E-3</v>
       </c>
       <c r="K2">
-        <f>'LDV psg'!K5</f>
-        <v>1.5777856020187898E-3</v>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!K$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.5814082719479863E-3</v>
       </c>
       <c r="L2">
-        <f>'LDV psg'!L5</f>
-        <v>1.5777856020187898E-3</v>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!L$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.5836470150648531E-3</v>
       </c>
       <c r="M2">
-        <f>'LDV psg'!M5</f>
-        <v>1.5772719898126412E-3</v>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!M$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.5878695012540782E-3</v>
       </c>
       <c r="N2">
-        <f>'LDV psg'!N5</f>
-        <v>1.5792887696596991E-3</v>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!N$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.5878695012540782E-3</v>
       </c>
       <c r="O2">
-        <f>'LDV psg'!O5</f>
-        <v>1.5814082719479863E-3</v>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!O$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.6168768200735936E-3</v>
       </c>
       <c r="P2">
-        <f>'LDV psg'!P5</f>
-        <v>1.5836470150648531E-3</v>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!P$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.6684754899028904E-3</v>
       </c>
       <c r="Q2">
-        <f>'LDV psg'!Q5</f>
-        <v>1.5878695012540782E-3</v>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!Q$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.6925103007190251E-3</v>
       </c>
       <c r="R2">
-        <f>'LDV psg'!R5</f>
-        <v>1.5878695012540782E-3</v>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!R$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.7311606219430804E-3</v>
       </c>
       <c r="S2">
-        <f>'LDV psg'!S5</f>
-        <v>1.6168768200735936E-3</v>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!S$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.7599919774426065E-3</v>
       </c>
       <c r="T2">
-        <f>'LDV psg'!T5</f>
-        <v>1.6684754899028904E-3</v>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!T$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.8032826149254849E-3</v>
       </c>
       <c r="U2">
-        <f>'LDV psg'!U5</f>
-        <v>1.6925103007190251E-3</v>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!U$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.8390205149056255E-3</v>
       </c>
       <c r="V2">
-        <f>'LDV psg'!V5</f>
-        <v>1.7311606219430804E-3</v>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!V$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.8682996654929781E-3</v>
       </c>
       <c r="W2">
-        <f>'LDV psg'!W5</f>
-        <v>1.7599919774426065E-3</v>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!W$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.9009085220263408E-3</v>
       </c>
       <c r="X2">
-        <f>'LDV psg'!X5</f>
-        <v>1.8032826149254849E-3</v>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!X$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.9488624245779288E-3</v>
       </c>
       <c r="Y2">
-        <f>'LDV psg'!Y5</f>
-        <v>1.8390205149056255E-3</v>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!Y$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.9736634876968292E-3</v>
       </c>
       <c r="Z2">
-        <f>'LDV psg'!Z5</f>
-        <v>1.8682996654929781E-3</v>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!Z$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.9987810231809769E-3</v>
       </c>
       <c r="AA2">
-        <f>'LDV psg'!AA5</f>
-        <v>1.9009085220263408E-3</v>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!AA$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>2.0242190800843275E-3</v>
       </c>
       <c r="AB2">
-        <f>'LDV psg'!AB5</f>
-        <v>1.9488624245779288E-3</v>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!AB$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>2.0499817597396139E-3</v>
       </c>
       <c r="AC2">
-        <f>'LDV psg'!AC5</f>
-        <v>1.9736634876968292E-3</v>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!AC$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>2.0760731939270297E-3</v>
       </c>
       <c r="AD2">
-        <f>'LDV psg'!AD5</f>
-        <v>1.9987810231809769E-3</v>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!AD$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>2.1024976455377448E-3</v>
       </c>
       <c r="AE2">
-        <f>'LDV psg'!AE5</f>
-        <v>2.0242190800843275E-3</v>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!AE$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>2.1292593051879484E-3</v>
       </c>
       <c r="AF2">
-        <f>'LDV psg'!AF5</f>
-        <v>2.0499817597396139E-3</v>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!AF$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>2.1563625406844388E-3</v>
       </c>
       <c r="AG2">
-        <f>'LDV psg'!AG5</f>
-        <v>2.0760731939270297E-3</v>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!AG$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>2.1838117041347036E-3</v>
       </c>
       <c r="AH2">
-        <f>'LDV psg'!AH5</f>
-        <v>2.1024976455377448E-3</v>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!AH$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>2.211611221543717E-3</v>
       </c>
       <c r="AI2">
-        <f>'LDV psg'!AI5</f>
-        <v>2.1292593051879484E-3</v>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!AI$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>2.2397655758389996E-3</v>
       </c>
       <c r="AJ2">
-        <f>'LDV psg'!AJ5</f>
-        <v>2.1563625406844388E-3</v>
+        <f>INDEX('LDV psg'!$B$5:$BA$5,1,MATCH('BHNVFEAL-LDVs-psgr'!AJ$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>2.2682793084371935E-3</v>
       </c>
     </row>
     <row r="3" spans="1:36">
@@ -15775,144 +15798,144 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <f>'LDV psg'!B3</f>
-        <v>3.1856391074337059E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!B$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>3.0411182142128833E-4</v>
       </c>
       <c r="C4">
-        <f>'LDV psg'!C3</f>
-        <v>3.0801370458911361E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!C$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>3.0108692529822541E-4</v>
       </c>
       <c r="D4">
-        <f>'LDV psg'!D3</f>
-        <v>3.0848299413300292E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!D$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>3.014263012403966E-4</v>
       </c>
       <c r="E4">
-        <f>'LDV psg'!E3</f>
-        <v>3.0661705462732352E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!E$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>3.0041638185002568E-4</v>
       </c>
       <c r="F4">
-        <f>'LDV psg'!F3</f>
-        <v>3.0411182142128833E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!F$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>3.0231143746099141E-4</v>
       </c>
       <c r="G4">
-        <f>'LDV psg'!G3</f>
-        <v>3.0108692529822541E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!G$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>3.0444438810792954E-4</v>
       </c>
       <c r="H4">
-        <f>'LDV psg'!H3</f>
-        <v>3.014263012403966E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!H$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>3.0832508399349155E-4</v>
       </c>
       <c r="I4">
-        <f>'LDV psg'!I3</f>
-        <v>3.0041638185002568E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!I$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>2.9086605032331933E-4</v>
       </c>
       <c r="J4">
-        <f>'LDV psg'!J3</f>
-        <v>3.0231143746099141E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!J$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>2.8972262451586384E-4</v>
       </c>
       <c r="K4">
-        <f>'LDV psg'!K3</f>
-        <v>3.0444438810792954E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!K$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>3.2496998697161418E-4</v>
       </c>
       <c r="L4">
-        <f>'LDV psg'!L3</f>
-        <v>3.0832508399349155E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!L$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>3.3461606145790266E-4</v>
       </c>
       <c r="M4">
-        <f>'LDV psg'!M3</f>
-        <v>2.9086605032331933E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!M$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>3.4503112454012272E-4</v>
       </c>
       <c r="N4">
-        <f>'LDV psg'!N3</f>
-        <v>2.8972262451586384E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!N$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>3.6046783839253731E-4</v>
       </c>
       <c r="O4">
-        <f>'LDV psg'!O3</f>
-        <v>3.2496998697161418E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!O$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>3.7661142322346664E-4</v>
       </c>
       <c r="P4">
-        <f>'LDV psg'!P3</f>
-        <v>3.3461606145790266E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!P$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>3.9323042596637155E-4</v>
       </c>
       <c r="Q4">
-        <f>'LDV psg'!Q3</f>
-        <v>3.4503112454012272E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!Q$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>4.0681862804371229E-4</v>
       </c>
       <c r="R4">
-        <f>'LDV psg'!R3</f>
-        <v>3.6046783839253731E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!R$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>4.2149750581699105E-4</v>
       </c>
       <c r="S4">
-        <f>'LDV psg'!S3</f>
-        <v>3.7661142322346664E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!S$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>4.3552727787002534E-4</v>
       </c>
       <c r="T4">
-        <f>'LDV psg'!T3</f>
-        <v>3.9323042596637155E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!T$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>4.5787211820594976E-4</v>
       </c>
       <c r="U4">
-        <f>'LDV psg'!U3</f>
-        <v>4.0681862804371229E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!U$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>4.7636139511923167E-4</v>
       </c>
       <c r="V4">
-        <f>'LDV psg'!V3</f>
-        <v>4.2149750581699105E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!V$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>4.9474731787187772E-4</v>
       </c>
       <c r="W4">
-        <f>'LDV psg'!W3</f>
-        <v>4.3552727787002534E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!W$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>5.1365533981639411E-4</v>
       </c>
       <c r="X4">
-        <f>'LDV psg'!X3</f>
-        <v>4.5787211820594976E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!X$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>5.4269272028124177E-4</v>
       </c>
       <c r="Y4">
-        <f>'LDV psg'!Y3</f>
-        <v>4.7636139511923167E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!Y$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>5.423016176547402E-4</v>
       </c>
       <c r="Z4">
-        <f>'LDV psg'!Z3</f>
-        <v>4.9474731787187772E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!Z$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>5.4224402286642641E-4</v>
       </c>
       <c r="AA4">
-        <f>'LDV psg'!AA3</f>
-        <v>5.1365533981639411E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!AA$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>5.4206760834494573E-4</v>
       </c>
       <c r="AB4">
-        <f>'LDV psg'!AB3</f>
-        <v>5.4269272028124177E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!AB$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>5.4189067774714969E-4</v>
       </c>
       <c r="AC4">
-        <f>'LDV psg'!AC3</f>
-        <v>5.423016176547402E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!AC$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>5.4171963799186189E-4</v>
       </c>
       <c r="AD4">
-        <f>'LDV psg'!AD3</f>
-        <v>5.4224402286642641E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!AD$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>5.4140776270668409E-4</v>
       </c>
       <c r="AE4">
-        <f>'LDV psg'!AE3</f>
-        <v>5.4206760834494573E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!AE$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>5.4295307935355247E-4</v>
       </c>
       <c r="AF4">
-        <f>'LDV psg'!AF3</f>
-        <v>5.4189067774714969E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!AF$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>5.4268045456530383E-4</v>
       </c>
       <c r="AG4">
-        <f>'LDV psg'!AG3</f>
-        <v>5.4171963799186189E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!AG$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>5.4251269578111186E-4</v>
       </c>
       <c r="AH4">
-        <f>'LDV psg'!AH3</f>
-        <v>5.4140776270668409E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!AH$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>5.4235202859305594E-4</v>
       </c>
       <c r="AI4">
-        <f>'LDV psg'!AI3</f>
-        <v>5.4295307935355247E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!AI$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>5.4218265683519029E-4</v>
       </c>
       <c r="AJ4">
-        <f>'LDV psg'!AJ3</f>
-        <v>5.4268045456530383E-4</v>
+        <f>INDEX('LDV psg'!$B$3:$BA$3,1,MATCH('BHNVFEAL-LDVs-psgr'!AJ$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>5.4203836899892029E-4</v>
       </c>
     </row>
     <row r="5" spans="1:36">
@@ -16030,144 +16053,144 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <f>'LDV psg'!B4</f>
-        <v>1.0111358409448513E-3</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!B$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.0046324007499143E-3</v>
       </c>
       <c r="C6">
-        <f>'LDV psg'!C4</f>
-        <v>1.0063882481754357E-3</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!C$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.0032711974945359E-3</v>
       </c>
       <c r="D6">
-        <f>'LDV psg'!D4</f>
-        <v>1.0065994284701859E-3</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!D$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.0034239166685128E-3</v>
       </c>
       <c r="E6">
-        <f>'LDV psg'!E4</f>
-        <v>1.0057597556926302E-3</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!E$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.002969452942846E-3</v>
       </c>
       <c r="F6">
-        <f>'LDV psg'!F4</f>
-        <v>1.0046324007499143E-3</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!F$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.0038222279677804E-3</v>
       </c>
       <c r="G6">
-        <f>'LDV psg'!G4</f>
-        <v>1.0032711974945359E-3</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!G$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.0047820557589028E-3</v>
       </c>
       <c r="H6">
-        <f>'LDV psg'!H4</f>
-        <v>1.0034239166685128E-3</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!H$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.0065283689074057E-3</v>
       </c>
       <c r="I6">
-        <f>'LDV psg'!I4</f>
-        <v>1.002969452942846E-3</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!I$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>9.9838931704244647E-4</v>
       </c>
       <c r="J6">
-        <f>'LDV psg'!J4</f>
-        <v>1.0038222279677804E-3</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!J$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>9.9898400434497345E-4</v>
       </c>
       <c r="K6">
-        <f>'LDV psg'!K4</f>
-        <v>1.0047820557589028E-3</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!K$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.016011043708619E-3</v>
       </c>
       <c r="L6">
-        <f>'LDV psg'!L4</f>
-        <v>1.0065283689074057E-3</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!L$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.0215830859417257E-3</v>
       </c>
       <c r="M6">
-        <f>'LDV psg'!M4</f>
-        <v>9.9838931704244647E-4</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!M$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.0285922317327984E-3</v>
       </c>
       <c r="N6">
-        <f>'LDV psg'!N4</f>
-        <v>9.9898400434497345E-4</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!N$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.0355387529663849E-3</v>
       </c>
       <c r="O6">
-        <f>'LDV psg'!O4</f>
-        <v>1.016011043708619E-3</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!O$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.0587573914910364E-3</v>
       </c>
       <c r="P6">
-        <f>'LDV psg'!P4</f>
-        <v>1.0215830859417257E-3</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!P$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.0946152111314569E-3</v>
       </c>
       <c r="Q6">
-        <f>'LDV psg'!Q4</f>
-        <v>1.0285922317327984E-3</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!Q$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.1139490480151345E-3</v>
       </c>
       <c r="R6">
-        <f>'LDV psg'!R4</f>
-        <v>1.0355387529663849E-3</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!R$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.1418122196863402E-3</v>
       </c>
       <c r="S6">
-        <f>'LDV psg'!S4</f>
-        <v>1.0587573914910364E-3</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!S$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.1639828626349451E-3</v>
       </c>
       <c r="T6">
-        <f>'LDV psg'!T4</f>
-        <v>1.0946152111314569E-3</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!T$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.1978478914016946E-3</v>
       </c>
       <c r="U6">
-        <f>'LDV psg'!U4</f>
-        <v>1.1139490480151345E-3</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!U$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.2258239110017482E-3</v>
       </c>
       <c r="V6">
-        <f>'LDV psg'!V4</f>
-        <v>1.1418122196863402E-3</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!V$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.2502011090634831E-3</v>
       </c>
       <c r="W6">
-        <f>'LDV psg'!W4</f>
-        <v>1.1639828626349451E-3</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!W$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.2766445900318649E-3</v>
       </c>
       <c r="X6">
-        <f>'LDV psg'!X4</f>
-        <v>1.1978478914016946E-3</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!X$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.3160860576444196E-3</v>
       </c>
       <c r="Y6">
-        <f>'LDV psg'!Y4</f>
-        <v>1.2258239110017482E-3</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!Y$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.3295506461778893E-3</v>
       </c>
       <c r="Z6">
-        <f>'LDV psg'!Z4</f>
-        <v>1.2502011090634831E-3</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!Z$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.343339373039429E-3</v>
       </c>
       <c r="AA6">
-        <f>'LDV psg'!AA4</f>
-        <v>1.2766445900318649E-3</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!AA$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.3572509178016059E-3</v>
       </c>
       <c r="AB6">
-        <f>'LDV psg'!AB4</f>
-        <v>1.3160860576444196E-3</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!AB$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.3713407728430051E-3</v>
       </c>
       <c r="AC6">
-        <f>'LDV psg'!AC4</f>
-        <v>1.3295506461778893E-3</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!AC$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.3856140937562043E-3</v>
       </c>
       <c r="AD6">
-        <f>'LDV psg'!AD4</f>
-        <v>1.343339373039429E-3</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!AD$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.4000071982637676E-3</v>
       </c>
       <c r="AE6">
-        <f>'LDV psg'!AE4</f>
-        <v>1.3572509178016059E-3</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!AE$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.4154215035624702E-3</v>
       </c>
       <c r="AF6">
-        <f>'LDV psg'!AF4</f>
-        <v>1.3713407728430051E-3</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!AF$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.4302056019308282E-3</v>
       </c>
       <c r="AG6">
-        <f>'LDV psg'!AG4</f>
-        <v>1.3856140937562043E-3</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!AG$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.4452271503755873E-3</v>
       </c>
       <c r="AH6">
-        <f>'LDV psg'!AH4</f>
-        <v>1.4000071982637676E-3</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!AH$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.4604445847159198E-3</v>
       </c>
       <c r="AI6">
-        <f>'LDV psg'!AI4</f>
-        <v>1.4154215035624702E-3</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!AI$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.4758532622872857E-3</v>
       </c>
       <c r="AJ6">
-        <f>'LDV psg'!AJ4</f>
-        <v>1.4302056019308282E-3</v>
+        <f>INDEX('LDV psg'!$B$4:$BA$4,1,MATCH('BHNVFEAL-LDVs-psgr'!AJ$1-About!$A$14,'LDV psg'!$B$2:$BA$2,0))</f>
+        <v>1.4914708856899707E-3</v>
       </c>
     </row>
     <row r="7" spans="1:36">

</xml_diff>